<commit_message>
limpieza y primeros exitos
</commit_message>
<xml_diff>
--- a/base_data.xlsx
+++ b/base_data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Master EIT\Madrid_UPM\Second Semester\Information Retrieval\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170FCD70-97C4-4CC8-BF7D-E9B215A2BE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF5CD5-983E-44F4-9836-E6899EF77E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36048" yWindow="3960" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="228">
   <si>
     <t>loinc_num</t>
   </si>
@@ -701,6 +702,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Y2</t>
   </si>
 </sst>
 </file>
@@ -765,7 +769,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -788,17 +792,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -806,7 +799,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -826,9 +819,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1134,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H202"/>
+  <dimension ref="A1:I202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C128" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136:H202"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1140,7 @@
     <col min="7" max="7" width="13.44140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>134</v>
       </c>
@@ -1172,11 +1162,14 @@
       <c r="G1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1201,8 +1194,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1227,8 +1223,11 @@
       <c r="H3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1253,8 +1252,11 @@
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1279,8 +1281,11 @@
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -1305,8 +1310,11 @@
       <c r="H6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1331,8 +1339,11 @@
       <c r="H7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -1357,8 +1368,11 @@
       <c r="H8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -1383,8 +1397,11 @@
       <c r="H9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1409,8 +1426,11 @@
       <c r="H10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1435,8 +1455,11 @@
       <c r="H11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1461,8 +1484,11 @@
       <c r="H12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1487,8 +1513,11 @@
       <c r="H13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1513,8 +1542,11 @@
       <c r="H14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -1539,8 +1571,11 @@
       <c r="H15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -1565,8 +1600,11 @@
       <c r="H16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -1591,8 +1629,11 @@
       <c r="H17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -1617,8 +1658,11 @@
       <c r="H18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -1643,8 +1687,11 @@
       <c r="H19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -1669,8 +1716,11 @@
       <c r="H20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -1695,8 +1745,11 @@
       <c r="H21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1721,8 +1774,11 @@
       <c r="H22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -1747,8 +1803,11 @@
       <c r="H23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>1</v>
       </c>
@@ -1773,8 +1832,11 @@
       <c r="H24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>1</v>
       </c>
@@ -1799,8 +1861,11 @@
       <c r="H25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>1</v>
       </c>
@@ -1825,8 +1890,11 @@
       <c r="H26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>1</v>
       </c>
@@ -1851,8 +1919,11 @@
       <c r="H27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>1</v>
       </c>
@@ -1877,8 +1948,11 @@
       <c r="H28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>1</v>
       </c>
@@ -1903,8 +1977,11 @@
       <c r="H29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1929,8 +2006,11 @@
       <c r="H30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>1</v>
       </c>
@@ -1955,8 +2035,11 @@
       <c r="H31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>1</v>
       </c>
@@ -1981,8 +2064,11 @@
       <c r="H32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>1</v>
       </c>
@@ -2007,8 +2093,11 @@
       <c r="H33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>1</v>
       </c>
@@ -2033,8 +2122,11 @@
       <c r="H34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -2059,8 +2151,11 @@
       <c r="H35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>1</v>
       </c>
@@ -2085,8 +2180,11 @@
       <c r="H36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>1</v>
       </c>
@@ -2111,8 +2209,11 @@
       <c r="H37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>1</v>
       </c>
@@ -2137,8 +2238,11 @@
       <c r="H38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>1</v>
       </c>
@@ -2163,8 +2267,11 @@
       <c r="H39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>1</v>
       </c>
@@ -2189,8 +2296,11 @@
       <c r="H40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>1</v>
       </c>
@@ -2215,8 +2325,11 @@
       <c r="H41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>1</v>
       </c>
@@ -2241,8 +2354,11 @@
       <c r="H42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -2267,8 +2383,11 @@
       <c r="H43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>1</v>
       </c>
@@ -2293,8 +2412,11 @@
       <c r="H44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>1</v>
       </c>
@@ -2319,8 +2441,11 @@
       <c r="H45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>1</v>
       </c>
@@ -2345,8 +2470,11 @@
       <c r="H46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -2371,8 +2499,11 @@
       <c r="H47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -2397,8 +2528,11 @@
       <c r="H48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>1</v>
       </c>
@@ -2423,8 +2557,11 @@
       <c r="H49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>1</v>
       </c>
@@ -2449,8 +2586,11 @@
       <c r="H50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>1</v>
       </c>
@@ -2475,8 +2615,11 @@
       <c r="H51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>1</v>
       </c>
@@ -2501,8 +2644,11 @@
       <c r="H52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>1</v>
       </c>
@@ -2527,8 +2673,11 @@
       <c r="H53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>1</v>
       </c>
@@ -2553,8 +2702,11 @@
       <c r="H54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>1</v>
       </c>
@@ -2579,8 +2731,11 @@
       <c r="H55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>1</v>
       </c>
@@ -2605,8 +2760,11 @@
       <c r="H56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>1</v>
       </c>
@@ -2631,8 +2789,11 @@
       <c r="H57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>1</v>
       </c>
@@ -2657,8 +2818,11 @@
       <c r="H58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>1</v>
       </c>
@@ -2683,8 +2847,11 @@
       <c r="H59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>1</v>
       </c>
@@ -2709,8 +2876,11 @@
       <c r="H60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>1</v>
       </c>
@@ -2735,8 +2905,11 @@
       <c r="H61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>1</v>
       </c>
@@ -2761,8 +2934,11 @@
       <c r="H62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>1</v>
       </c>
@@ -2787,8 +2963,11 @@
       <c r="H63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>1</v>
       </c>
@@ -2813,8 +2992,11 @@
       <c r="H64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>1</v>
       </c>
@@ -2839,8 +3021,11 @@
       <c r="H65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>1</v>
       </c>
@@ -2865,8 +3050,11 @@
       <c r="H66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>1</v>
       </c>
@@ -2891,8 +3079,11 @@
       <c r="H67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>1</v>
       </c>
@@ -2917,8 +3108,11 @@
       <c r="H68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>2</v>
       </c>
@@ -2943,8 +3137,11 @@
       <c r="H69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>2</v>
       </c>
@@ -2969,8 +3166,11 @@
       <c r="H70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>2</v>
       </c>
@@ -2995,8 +3195,11 @@
       <c r="H71">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>2</v>
       </c>
@@ -3021,8 +3224,11 @@
       <c r="H72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>2</v>
       </c>
@@ -3047,8 +3253,11 @@
       <c r="H73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>2</v>
       </c>
@@ -3073,8 +3282,11 @@
       <c r="H74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>2</v>
       </c>
@@ -3099,8 +3311,11 @@
       <c r="H75">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>2</v>
       </c>
@@ -3125,8 +3340,11 @@
       <c r="H76">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>2</v>
       </c>
@@ -3151,8 +3369,11 @@
       <c r="H77">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>2</v>
       </c>
@@ -3177,8 +3398,11 @@
       <c r="H78">
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>2</v>
       </c>
@@ -3203,8 +3427,11 @@
       <c r="H79">
         <v>11</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>2</v>
       </c>
@@ -3229,8 +3456,11 @@
       <c r="H80">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>2</v>
       </c>
@@ -3255,8 +3485,11 @@
       <c r="H81">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>2</v>
       </c>
@@ -3281,8 +3514,11 @@
       <c r="H82">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>2</v>
       </c>
@@ -3307,8 +3543,11 @@
       <c r="H83">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>2</v>
       </c>
@@ -3333,8 +3572,11 @@
       <c r="H84">
         <v>16</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>2</v>
       </c>
@@ -3359,8 +3601,11 @@
       <c r="H85">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>2</v>
       </c>
@@ -3385,8 +3630,11 @@
       <c r="H86">
         <v>18</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>2</v>
       </c>
@@ -3411,8 +3659,11 @@
       <c r="H87">
         <v>19</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>2</v>
       </c>
@@ -3437,8 +3688,11 @@
       <c r="H88">
         <v>20</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>2</v>
       </c>
@@ -3463,8 +3717,11 @@
       <c r="H89">
         <v>21</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>2</v>
       </c>
@@ -3489,8 +3746,11 @@
       <c r="H90">
         <v>22</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>2</v>
       </c>
@@ -3515,8 +3775,11 @@
       <c r="H91">
         <v>23</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>2</v>
       </c>
@@ -3541,8 +3804,11 @@
       <c r="H92">
         <v>24</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>2</v>
       </c>
@@ -3567,8 +3833,11 @@
       <c r="H93">
         <v>25</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>2</v>
       </c>
@@ -3593,8 +3862,11 @@
       <c r="H94">
         <v>26</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>2</v>
       </c>
@@ -3619,8 +3891,11 @@
       <c r="H95">
         <v>27</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>2</v>
       </c>
@@ -3645,8 +3920,11 @@
       <c r="H96">
         <v>28</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>2</v>
       </c>
@@ -3671,8 +3949,11 @@
       <c r="H97">
         <v>29</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>2</v>
       </c>
@@ -3697,8 +3978,11 @@
       <c r="H98">
         <v>30</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>2</v>
       </c>
@@ -3723,8 +4007,11 @@
       <c r="H99">
         <v>31</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>2</v>
       </c>
@@ -3749,8 +4036,11 @@
       <c r="H100">
         <v>32</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>2</v>
       </c>
@@ -3775,8 +4065,11 @@
       <c r="H101">
         <v>33</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>2</v>
       </c>
@@ -3801,8 +4094,11 @@
       <c r="H102">
         <v>34</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>2</v>
       </c>
@@ -3827,8 +4123,11 @@
       <c r="H103">
         <v>35</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>2</v>
       </c>
@@ -3853,8 +4152,11 @@
       <c r="H104">
         <v>36</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>2</v>
       </c>
@@ -3879,8 +4181,11 @@
       <c r="H105">
         <v>37</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>2</v>
       </c>
@@ -3905,8 +4210,11 @@
       <c r="H106">
         <v>38</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>2</v>
       </c>
@@ -3931,8 +4239,11 @@
       <c r="H107">
         <v>39</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>2</v>
       </c>
@@ -3957,8 +4268,11 @@
       <c r="H108">
         <v>40</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>2</v>
       </c>
@@ -3983,8 +4297,11 @@
       <c r="H109">
         <v>41</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>2</v>
       </c>
@@ -4009,8 +4326,11 @@
       <c r="H110">
         <v>42</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>2</v>
       </c>
@@ -4035,8 +4355,11 @@
       <c r="H111">
         <v>43</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>2</v>
       </c>
@@ -4061,8 +4384,11 @@
       <c r="H112">
         <v>44</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="5">
         <v>2</v>
       </c>
@@ -4087,8 +4413,11 @@
       <c r="H113">
         <v>45</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
         <v>2</v>
       </c>
@@ -4113,8 +4442,11 @@
       <c r="H114">
         <v>46</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>2</v>
       </c>
@@ -4139,8 +4471,11 @@
       <c r="H115">
         <v>47</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="5">
         <v>2</v>
       </c>
@@ -4165,8 +4500,11 @@
       <c r="H116">
         <v>48</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="5">
         <v>2</v>
       </c>
@@ -4191,8 +4529,11 @@
       <c r="H117">
         <v>49</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="5">
         <v>2</v>
       </c>
@@ -4217,8 +4558,11 @@
       <c r="H118">
         <v>50</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="5">
         <v>2</v>
       </c>
@@ -4243,8 +4587,11 @@
       <c r="H119">
         <v>51</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="5">
         <v>2</v>
       </c>
@@ -4269,8 +4616,11 @@
       <c r="H120">
         <v>52</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="5">
         <v>2</v>
       </c>
@@ -4295,8 +4645,11 @@
       <c r="H121">
         <v>53</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="5">
         <v>2</v>
       </c>
@@ -4321,8 +4674,11 @@
       <c r="H122">
         <v>54</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="5">
         <v>2</v>
       </c>
@@ -4347,8 +4703,11 @@
       <c r="H123">
         <v>55</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="5">
         <v>2</v>
       </c>
@@ -4373,8 +4732,11 @@
       <c r="H124">
         <v>56</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="5">
         <v>2</v>
       </c>
@@ -4399,8 +4761,11 @@
       <c r="H125">
         <v>57</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="5">
         <v>2</v>
       </c>
@@ -4425,8 +4790,11 @@
       <c r="H126">
         <v>58</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="5">
         <v>2</v>
       </c>
@@ -4451,8 +4819,11 @@
       <c r="H127">
         <v>59</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="5">
         <v>2</v>
       </c>
@@ -4477,8 +4848,11 @@
       <c r="H128">
         <v>60</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="5">
         <v>2</v>
       </c>
@@ -4503,8 +4877,11 @@
       <c r="H129">
         <v>61</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="5">
         <v>2</v>
       </c>
@@ -4529,8 +4906,11 @@
       <c r="H130">
         <v>62</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="5">
         <v>2</v>
       </c>
@@ -4555,8 +4935,11 @@
       <c r="H131">
         <v>63</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="5">
         <v>2</v>
       </c>
@@ -4581,8 +4964,11 @@
       <c r="H132">
         <v>64</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="5">
         <v>2</v>
       </c>
@@ -4607,8 +4993,11 @@
       <c r="H133">
         <v>65</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="5">
         <v>2</v>
       </c>
@@ -4633,8 +5022,11 @@
       <c r="H134">
         <v>66</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="5">
         <v>2</v>
       </c>
@@ -4659,8 +5051,11 @@
       <c r="H135">
         <v>67</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="7">
         <v>3</v>
       </c>
@@ -4685,8 +5080,11 @@
       <c r="H136">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="7">
         <v>3</v>
       </c>
@@ -4711,8 +5109,11 @@
       <c r="H137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="7">
         <v>3</v>
       </c>
@@ -4737,8 +5138,11 @@
       <c r="H138">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="7">
         <v>3</v>
       </c>
@@ -4763,8 +5167,11 @@
       <c r="H139">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="7">
         <v>3</v>
       </c>
@@ -4789,8 +5196,11 @@
       <c r="H140">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="7">
         <v>3</v>
       </c>
@@ -4815,8 +5225,11 @@
       <c r="H141">
         <v>6</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="7">
         <v>3</v>
       </c>
@@ -4841,8 +5254,11 @@
       <c r="H142">
         <v>7</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="7">
         <v>3</v>
       </c>
@@ -4867,8 +5283,11 @@
       <c r="H143">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="7">
         <v>3</v>
       </c>
@@ -4893,8 +5312,11 @@
       <c r="H144">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
         <v>3</v>
       </c>
@@ -4919,8 +5341,11 @@
       <c r="H145">
         <v>10</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="7">
         <v>3</v>
       </c>
@@ -4945,8 +5370,11 @@
       <c r="H146">
         <v>11</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="7">
         <v>3</v>
       </c>
@@ -4971,8 +5399,11 @@
       <c r="H147">
         <v>12</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
         <v>3</v>
       </c>
@@ -4997,8 +5428,11 @@
       <c r="H148">
         <v>13</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="7">
         <v>3</v>
       </c>
@@ -5023,8 +5457,11 @@
       <c r="H149">
         <v>14</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="7">
         <v>3</v>
       </c>
@@ -5049,8 +5486,11 @@
       <c r="H150">
         <v>15</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="7">
         <v>3</v>
       </c>
@@ -5075,8 +5515,11 @@
       <c r="H151">
         <v>16</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="7">
         <v>3</v>
       </c>
@@ -5101,8 +5544,11 @@
       <c r="H152">
         <v>17</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="7">
         <v>3</v>
       </c>
@@ -5127,8 +5573,11 @@
       <c r="H153">
         <v>18</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="7">
         <v>3</v>
       </c>
@@ -5153,8 +5602,11 @@
       <c r="H154">
         <v>19</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="7">
         <v>3</v>
       </c>
@@ -5179,8 +5631,11 @@
       <c r="H155">
         <v>20</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="7">
         <v>3</v>
       </c>
@@ -5205,8 +5660,11 @@
       <c r="H156">
         <v>21</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="7">
         <v>3</v>
       </c>
@@ -5231,8 +5689,11 @@
       <c r="H157">
         <v>22</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="7">
         <v>3</v>
       </c>
@@ -5257,8 +5718,11 @@
       <c r="H158">
         <v>23</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="7">
         <v>3</v>
       </c>
@@ -5283,8 +5747,11 @@
       <c r="H159">
         <v>24</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="7">
         <v>3</v>
       </c>
@@ -5309,8 +5776,11 @@
       <c r="H160">
         <v>25</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="7">
         <v>3</v>
       </c>
@@ -5335,8 +5805,11 @@
       <c r="H161">
         <v>26</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="7">
         <v>3</v>
       </c>
@@ -5361,8 +5834,11 @@
       <c r="H162">
         <v>27</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="7">
         <v>3</v>
       </c>
@@ -5387,8 +5863,11 @@
       <c r="H163">
         <v>28</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="7">
         <v>3</v>
       </c>
@@ -5413,8 +5892,11 @@
       <c r="H164">
         <v>29</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="7">
         <v>3</v>
       </c>
@@ -5439,8 +5921,11 @@
       <c r="H165">
         <v>30</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="7">
         <v>3</v>
       </c>
@@ -5465,8 +5950,11 @@
       <c r="H166">
         <v>31</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="7">
         <v>3</v>
       </c>
@@ -5491,8 +5979,11 @@
       <c r="H167">
         <v>32</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="7">
         <v>3</v>
       </c>
@@ -5517,8 +6008,11 @@
       <c r="H168">
         <v>33</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="7">
         <v>3</v>
       </c>
@@ -5543,8 +6037,11 @@
       <c r="H169">
         <v>34</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="7">
         <v>3</v>
       </c>
@@ -5569,8 +6066,11 @@
       <c r="H170">
         <v>35</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="7">
         <v>3</v>
       </c>
@@ -5595,8 +6095,11 @@
       <c r="H171">
         <v>36</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="7">
         <v>3</v>
       </c>
@@ -5621,8 +6124,11 @@
       <c r="H172">
         <v>37</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="7">
         <v>3</v>
       </c>
@@ -5647,8 +6153,11 @@
       <c r="H173">
         <v>38</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="7">
         <v>3</v>
       </c>
@@ -5673,8 +6182,11 @@
       <c r="H174">
         <v>39</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="7">
         <v>3</v>
       </c>
@@ -5699,8 +6211,11 @@
       <c r="H175">
         <v>40</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="7">
         <v>3</v>
       </c>
@@ -5725,8 +6240,11 @@
       <c r="H176">
         <v>41</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" s="7">
         <v>3</v>
       </c>
@@ -5751,8 +6269,11 @@
       <c r="H177">
         <v>42</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="7">
         <v>3</v>
       </c>
@@ -5777,8 +6298,11 @@
       <c r="H178">
         <v>43</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="7">
         <v>3</v>
       </c>
@@ -5803,8 +6327,11 @@
       <c r="H179">
         <v>44</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="7">
         <v>3</v>
       </c>
@@ -5829,8 +6356,11 @@
       <c r="H180">
         <v>45</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="7">
         <v>3</v>
       </c>
@@ -5855,8 +6385,11 @@
       <c r="H181">
         <v>46</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="7">
         <v>3</v>
       </c>
@@ -5881,8 +6414,11 @@
       <c r="H182">
         <v>47</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="7">
         <v>3</v>
       </c>
@@ -5907,8 +6443,11 @@
       <c r="H183">
         <v>48</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="7">
         <v>3</v>
       </c>
@@ -5933,8 +6472,11 @@
       <c r="H184">
         <v>49</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="7">
         <v>3</v>
       </c>
@@ -5959,8 +6501,11 @@
       <c r="H185">
         <v>50</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="7">
         <v>3</v>
       </c>
@@ -5985,8 +6530,11 @@
       <c r="H186">
         <v>51</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="7">
         <v>3</v>
       </c>
@@ -6011,8 +6559,11 @@
       <c r="H187">
         <v>52</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="7">
         <v>3</v>
       </c>
@@ -6037,8 +6588,11 @@
       <c r="H188">
         <v>53</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="7">
         <v>3</v>
       </c>
@@ -6063,8 +6617,11 @@
       <c r="H189">
         <v>54</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="7">
         <v>3</v>
       </c>
@@ -6089,8 +6646,11 @@
       <c r="H190">
         <v>55</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="7">
         <v>3</v>
       </c>
@@ -6115,8 +6675,11 @@
       <c r="H191">
         <v>56</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="7">
         <v>3</v>
       </c>
@@ -6141,8 +6704,11 @@
       <c r="H192">
         <v>57</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="7">
         <v>3</v>
       </c>
@@ -6167,8 +6733,11 @@
       <c r="H193">
         <v>58</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="7">
         <v>3</v>
       </c>
@@ -6193,8 +6762,11 @@
       <c r="H194">
         <v>59</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="7">
         <v>3</v>
       </c>
@@ -6219,8 +6791,11 @@
       <c r="H195">
         <v>60</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="7">
         <v>3</v>
       </c>
@@ -6245,8 +6820,11 @@
       <c r="H196">
         <v>61</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="7">
         <v>3</v>
       </c>
@@ -6271,8 +6849,11 @@
       <c r="H197">
         <v>62</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="7">
         <v>3</v>
       </c>
@@ -6297,8 +6878,11 @@
       <c r="H198">
         <v>63</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="7">
         <v>3</v>
       </c>
@@ -6323,8 +6907,11 @@
       <c r="H199">
         <v>64</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="7">
         <v>3</v>
       </c>
@@ -6349,8 +6936,11 @@
       <c r="H200">
         <v>65</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="7">
         <v>3</v>
       </c>
@@ -6375,8 +6965,11 @@
       <c r="H201">
         <v>66</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="7">
         <v>3</v>
       </c>
@@ -6400,9 +6993,1598 @@
       </c>
       <c r="H202">
         <v>67</v>
+      </c>
+      <c r="I202">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E09ABB-74CB-40D9-8161-E5524986D2F6}">
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>47</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7">
+        <v>49</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="7">
+        <v>59</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="7">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="7">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7">
+        <v>57</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="7">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="7">
+        <v>41</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="7">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="7">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7">
+        <v>67</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="7">
+        <v>55</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="7">
+        <v>62</v>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="7">
+        <v>58</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="7">
+        <v>60</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="7">
+        <v>61</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="7">
+        <v>54</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="7">
+        <v>29</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="7">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="7">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>26</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="7">
+        <v>42</v>
+      </c>
+      <c r="F28">
+        <v>27</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="7">
+        <v>36</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="7">
+        <v>21</v>
+      </c>
+      <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="7">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="7">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>31</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="7">
+        <v>40</v>
+      </c>
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="7">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>33</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="7">
+        <v>35</v>
+      </c>
+      <c r="F35">
+        <v>34</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="7">
+        <v>14</v>
+      </c>
+      <c r="F36">
+        <v>35</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="7">
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <v>36</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="7">
+        <v>63</v>
+      </c>
+      <c r="F38">
+        <v>37</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="7">
+        <v>24</v>
+      </c>
+      <c r="F39">
+        <v>38</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="7">
+        <v>26</v>
+      </c>
+      <c r="F40">
+        <v>39</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="7">
+        <v>17</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="7">
+        <v>32</v>
+      </c>
+      <c r="F42">
+        <v>41</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="7">
+        <v>25</v>
+      </c>
+      <c r="F43">
+        <v>42</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="7">
+        <v>28</v>
+      </c>
+      <c r="F44">
+        <v>43</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="7">
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>44</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="7">
+        <v>53</v>
+      </c>
+      <c r="F46">
+        <v>45</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>46</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="7">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>47</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="7">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>48</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="7">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>49</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="7">
+        <v>11</v>
+      </c>
+      <c r="F51">
+        <v>50</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="7">
+        <v>46</v>
+      </c>
+      <c r="F52">
+        <v>51</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="7">
+        <v>45</v>
+      </c>
+      <c r="F53">
+        <v>52</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="7">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>53</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="7">
+        <v>51</v>
+      </c>
+      <c r="F55">
+        <v>54</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="7">
+        <v>16</v>
+      </c>
+      <c r="F56">
+        <v>55</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="7">
+        <v>43</v>
+      </c>
+      <c r="F57">
+        <v>56</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="7">
+        <v>23</v>
+      </c>
+      <c r="F58">
+        <v>57</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="7">
+        <v>64</v>
+      </c>
+      <c r="F59">
+        <v>58</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="7">
+        <v>37</v>
+      </c>
+      <c r="F60">
+        <v>59</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="7">
+        <v>39</v>
+      </c>
+      <c r="F61">
+        <v>60</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" s="7">
+        <v>65</v>
+      </c>
+      <c r="F62">
+        <v>61</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="7">
+        <v>48</v>
+      </c>
+      <c r="F63">
+        <v>62</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="7">
+        <v>44</v>
+      </c>
+      <c r="F64">
+        <v>63</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="7">
+        <v>6</v>
+      </c>
+      <c r="F65">
+        <v>64</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="7">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>65</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="7">
+        <v>27</v>
+      </c>
+      <c r="F67">
+        <v>66</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" s="7">
+        <v>8</v>
+      </c>
+      <c r="F68">
+        <v>67</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G68">
+    <sortCondition ref="F2:F68"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>